<commit_message>
basic functioning now completed. Correctly declares winners in basic scenario
</commit_message>
<xml_diff>
--- a/presidential.xlsx
+++ b/presidential.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Primary Vote" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Primary Vote" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Count_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Count_3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+  <si>
+    <t>Position</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -55,57 +60,61 @@
     <t>A</t>
   </si>
   <si>
+    <t>Jacky He</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
+    <t>Chia-shuo (Alex) Yang</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
+    <t>Adriana Malavisi</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
-    <t>Jacky</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Adriana</t>
-  </si>
-  <si>
-    <t>Lara</t>
+    <t>Lara Sonnenschein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -128,21 +137,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -430,84 +448,550 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="n">
+        <v>74</v>
+      </c>
+      <c r="D2" t="n">
+        <v>471</v>
+      </c>
+      <c r="E2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F2" t="n">
+        <v>71</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8</v>
+      </c>
+      <c r="K2" t="n">
         <v>12</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="n">
+        <v>161</v>
+      </c>
+      <c r="D3" t="n">
+        <v>266</v>
+      </c>
+      <c r="E3" t="n">
+        <v>305</v>
+      </c>
+      <c r="F3" t="n">
+        <v>141</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" t="n">
+        <v>4</v>
+      </c>
+      <c r="K3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="n">
+        <v>138</v>
+      </c>
+      <c r="D4" t="n">
+        <v>155</v>
+      </c>
+      <c r="E4" t="n">
+        <v>17</v>
+      </c>
+      <c r="F4" t="n">
+        <v>136</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8</v>
+      </c>
+      <c r="H4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="n">
+        <v>32</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="n">
+        <v>109</v>
+      </c>
+      <c r="D5" t="n">
+        <v>268</v>
+      </c>
+      <c r="E5" t="n">
+        <v>345</v>
+      </c>
+      <c r="F5" t="n">
+        <v>69</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" t="n">
+        <v>7</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="n">
+        <v>74</v>
+      </c>
+      <c r="D2" t="n">
+        <v>471</v>
+      </c>
+      <c r="E2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F2" t="n">
+        <v>71</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8</v>
+      </c>
+      <c r="K2" t="n">
+        <v>12</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="n">
+        <v>161</v>
+      </c>
+      <c r="D3" t="n">
+        <v>266</v>
+      </c>
+      <c r="E3" t="n">
+        <v>305</v>
+      </c>
+      <c r="F3" t="n">
+        <v>141</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" t="n">
+        <v>4</v>
+      </c>
+      <c r="K3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>109</v>
+      </c>
+      <c r="D4" t="n">
+        <v>268</v>
+      </c>
+      <c r="E4" t="n">
+        <v>345</v>
+      </c>
+      <c r="F4" t="n">
+        <v>69</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" t="n">
+        <v>7</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>806</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
+      <c r="C2" t="n">
+        <v>161</v>
+      </c>
+      <c r="D2" t="n">
+        <v>266</v>
+      </c>
+      <c r="E2" t="n">
+        <v>305</v>
+      </c>
+      <c r="F2" t="n">
+        <v>141</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>900</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
+      <c r="A3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>109</v>
+      </c>
+      <c r="D3" t="n">
+        <v>268</v>
+      </c>
+      <c r="E3" t="n">
+        <v>345</v>
+      </c>
+      <c r="F3" t="n">
+        <v>69</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" t="n">
+        <v>7</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>806</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>